<commit_message>
minor update to minimal templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/Assay_GEO_minimal.xlsx
+++ b/templates/dataplant/Assay_GEO_minimal.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\SWATE_templates\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D60090-CF87-4B2D-B3D7-2251D2ACB9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFAFDA5-CE68-452B-8F60-1FA88215B98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9075" yWindow="5100" windowWidth="22545" windowHeight="14295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="3ASY01_RNASeq" sheetId="1" r:id="rId1"/>
+    <sheet name="Assay" sheetId="1" r:id="rId1"/>
     <sheet name="SwateTemplateMetadata" sheetId="4" r:id="rId2"/>
     <sheet name="GEO_RNASEQ" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -292,9 +292,6 @@
     <t>Authors Affiliation</t>
   </si>
   <si>
-    <t>annotationTableSpicySloth85</t>
-  </si>
-  <si>
     <t>GEO</t>
   </si>
   <si>
@@ -738,6 +735,9 @@
   </si>
   <si>
     <t>PROTOCOLS_data processing step</t>
+  </si>
+  <si>
+    <t>annotationTableSpicySloth84</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1054,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8CF88B-39F4-4BB8-A79A-D46E92AF4094}" name="annotationTableSpicySloth85" displayName="annotationTableSpicySloth85" ref="A1:AJ5" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8CF88B-39F4-4BB8-A79A-D46E92AF4094}" name="annotationTableSpicySloth84" displayName="annotationTableSpicySloth84" ref="A1:AJ5" totalsRowShown="0">
   <autoFilter ref="A1:AJ5" xr:uid="{FF8CF88B-39F4-4BB8-A79A-D46E92AF4094}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{DDD81922-E978-4A5A-A247-30D8EC830850}" name="Source Name"/>
@@ -1429,7 +1429,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1487,22 +1489,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
         <v>126</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>127</v>
       </c>
-      <c r="D1" t="s">
-        <v>128</v>
-      </c>
       <c r="E1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" t="s">
         <v>131</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" t="s">
-        <v>133</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1553,13 +1555,13 @@
         <v>21</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Y1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z1" t="s">
         <v>101</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>102</v>
       </c>
       <c r="AA1" s="13" t="s">
         <v>22</v>
@@ -1589,140 +1591,140 @@
         <v>30</v>
       </c>
       <c r="AJ1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>97</v>
-      </c>
       <c r="Y2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA2" s="13"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -1737,59 +1739,59 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1804,13 +1806,13 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
@@ -1819,29 +1821,29 @@
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1875,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA628F8D-856A-498A-8154-924F19E80D38}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1892,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1898,7 +1900,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1906,7 +1908,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1914,7 +1916,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1922,7 +1924,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1930,7 +1932,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1944,7 +1946,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1952,7 +1954,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1960,7 +1962,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1974,19 +1976,19 @@
         <v>42</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,7 +2014,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2020,7 +2022,7 @@
         <v>47</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2034,7 +2036,7 @@
         <v>49</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2060,30 +2062,30 @@
         <v>53</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" s="10"/>
     </row>
@@ -2097,7 +2099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -2119,40 +2121,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2160,13 +2162,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -2179,36 +2181,36 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2216,29 +2218,29 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>139</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
@@ -2248,29 +2250,29 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>141</v>
-      </c>
       <c r="E5" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
@@ -2280,29 +2282,29 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
@@ -2312,31 +2314,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>142</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2344,27 +2346,27 @@
         <v>9</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>145</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="I8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
@@ -2374,27 +2376,27 @@
         <v>10</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>147</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="I9" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -2404,29 +2406,29 @@
         <v>11</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="E10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
@@ -2436,27 +2438,27 @@
         <v>15</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -2466,27 +2468,27 @@
         <v>16</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>152</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>153</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I12" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -2496,64 +2498,64 @@
         <v>19</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>155</v>
-      </c>
       <c r="E13" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H13" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="J13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>157</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H14" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="J14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="L14" s="12"/>
     </row>
@@ -2562,30 +2564,30 @@
         <v>22</v>
       </c>
       <c r="B15" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>158</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>159</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H15" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="J15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="L15" s="12"/>
     </row>
@@ -2594,27 +2596,27 @@
         <v>25</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>160</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>161</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="J16" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
@@ -2624,55 +2626,55 @@
         <v>28</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>162</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>163</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>

</xml_diff>